<commit_message>
get underway TOI GPS and edit project node
</commit_message>
<xml_diff>
--- a/ncp-gop-transect-2019-pkg14/ncp-gop-transect-2019-info.xlsx
+++ b/ncp-gop-transect-2019-pkg14/ncp-gop-transect-2019-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\ncp-gop-transect-2019-pkg14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E003BBE-9AD2-4635-9BF0-E8A716AF53AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD7661A-F9F6-4CD5-9E28-71CBE2A3BDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28845" yWindow="7995" windowWidth="28530" windowHeight="9360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersGop" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="120">
   <si>
     <t>givenName</t>
   </si>
@@ -143,18 +143,6 @@
     <t>primary production</t>
   </si>
   <si>
-    <t>Kate</t>
-  </si>
-  <si>
-    <t>Morkeski</t>
-  </si>
-  <si>
-    <t>kmorkeski@whoi.edu</t>
-  </si>
-  <si>
-    <t>0000-0002-2903-5851</t>
-  </si>
-  <si>
     <t>attributeName</t>
   </si>
   <si>
@@ -210,9 +198,6 @@
   </si>
   <si>
     <t>gross primary production</t>
-  </si>
-  <si>
-    <t>metadata Provider</t>
   </si>
   <si>
     <t>PI</t>
@@ -414,7 +399,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,13 +411,6 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF1D1C1D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -478,19 +456,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -821,202 +798,202 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>88</v>
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1041,160 +1018,160 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>88</v>
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1215,90 +1192,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1308,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1372,7 +1349,7 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1380,7 +1357,7 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1412,7 +1389,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -1444,7 +1421,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1459,7 +1436,7 @@
         <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -1482,7 +1459,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -1499,22 +1476,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>40</v>
+      <c r="E7" t="s">
+        <v>103</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -1523,22 +1497,19 @@
         <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>124</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
-        <v>108</v>
-      </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
@@ -1554,10 +1525,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1572,29 +1543,6 @@
         <v>12</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1604,10 +1552,9 @@
     <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1643,7 +1590,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1675,7 +1622,7 @@
     </row>
     <row r="7" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -1683,20 +1630,20 @@
     </row>
     <row r="8" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1738,16 +1685,16 @@
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="7">
+        <v>104</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="6">
         <v>1.1574070000000001E-8</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update project node, allow for new ncp columns
</commit_message>
<xml_diff>
--- a/ncp-gop-transect-2019-pkg14/ncp-gop-transect-2019-info.xlsx
+++ b/ncp-gop-transect-2019-pkg14/ncp-gop-transect-2019-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\ncp-gop-transect-2019-pkg14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD7661A-F9F6-4CD5-9E28-71CBE2A3BDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6346F12-1BDC-4E25-9050-5771FFDD2133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeadersGop" sheetId="7" r:id="rId1"/>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1476,17 +1476,14 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
-        <v>103</v>
-      </c>
       <c r="G7" t="s">
         <v>11</v>
       </c>
@@ -1502,14 +1499,17 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
@@ -1525,10 +1525,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>

</xml_diff>